<commit_message>
Updated stepper timer calculations.
</commit_message>
<xml_diff>
--- a/DOC/Stepper_timer_calculations.xlsx
+++ b/DOC/Stepper_timer_calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Git dev\SteppermotorController\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0297EE00-CBB7-4252-9325-AD9C47A18BB2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C651044-EC88-4143-8797-CDB35935E126}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{AF9EBE77-4D09-42D9-8DEF-F11C240E38CE}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -102,7 +103,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -110,29 +111,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -449,7 +427,7 @@
   <dimension ref="B1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="E1">
-        <v>3000000</v>
+        <v>12000000</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
@@ -564,79 +542,79 @@
       </c>
       <c r="F6">
         <f>($E$1 * 60 / ($D6*$E$2*F$4))</f>
-        <v>900000</v>
+        <v>3600000</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:V11" si="0">($E$1 * 60 / ($D6*$E$2*G$4))</f>
+        <v>1800000</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1200000</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>900000</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>720000</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>514285.71428571426</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
         <v>450000</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>225000</v>
-      </c>
-      <c r="J6">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>360000</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="0"/>
         <v>180000</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>150000</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>128571.42857142857</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>112500</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>90000</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>45000</v>
-      </c>
       <c r="Q6">
         <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-      <c r="R6">
+      <c r="V6">
         <f t="shared" si="0"/>
         <v>18000</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="0"/>
-        <v>15000</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="0"/>
-        <v>9000</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="0"/>
-        <v>7500</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="0"/>
-        <v>4500</v>
       </c>
       <c r="W6">
         <f t="shared" ref="V6:X11" si="1">($E$1 * 60 / ($D6*$E$2*W$4))</f>
-        <v>3750</v>
+        <v>15000</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
@@ -649,79 +627,79 @@
       </c>
       <c r="F7">
         <f t="shared" ref="F7:V11" si="3">($E$1 * 60 / ($D7*$E$2*F$4))</f>
+        <v>1800000</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>900000</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>600000</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
         <v>450000</v>
       </c>
-      <c r="G7">
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>360000</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>300000</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>257142.85714285713</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="3"/>
         <v>225000</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="3"/>
-        <v>150000</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
-        <v>112500</v>
-      </c>
-      <c r="J7">
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>200000</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>180000</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="3"/>
         <v>90000</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>75000</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="3"/>
-        <v>64285.714285714283</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>56250</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="3"/>
-        <v>50000</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="3"/>
-        <v>45000</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="3"/>
-        <v>22500</v>
-      </c>
       <c r="Q7">
         <f t="shared" si="3"/>
+        <v>60000</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>36000</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>30000</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>18000</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="3"/>
         <v>15000</v>
       </c>
-      <c r="R7">
+      <c r="V7">
         <f t="shared" si="3"/>
         <v>9000</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="3"/>
+      <c r="W7">
+        <f t="shared" si="1"/>
         <v>7500</v>
       </c>
-      <c r="T7">
-        <f t="shared" si="3"/>
-        <v>4500</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="3"/>
-        <v>3750</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="3"/>
-        <v>2250</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="1"/>
-        <v>1875</v>
-      </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
@@ -734,79 +712,79 @@
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
+        <v>900000</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>450000</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
         <v>225000</v>
       </c>
-      <c r="G8">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>180000</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>128571.42857142857</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>112500</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>75000</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>56250</v>
-      </c>
-      <c r="J8">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="0"/>
         <v>45000</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>37500</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>32142.857142857141</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>28125</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>25000</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>22500</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>11250</v>
-      </c>
       <c r="Q8">
         <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
         <v>7500</v>
       </c>
-      <c r="R8">
-        <f t="shared" si="0"/>
+      <c r="V8">
+        <f t="shared" si="1"/>
         <v>4500</v>
       </c>
-      <c r="S8">
-        <f t="shared" si="0"/>
+      <c r="W8">
+        <f t="shared" si="1"/>
         <v>3750</v>
       </c>
-      <c r="T8">
-        <f t="shared" si="0"/>
-        <v>2250</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="0"/>
-        <v>1875</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="1"/>
-        <v>1125</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="1"/>
-        <v>937.5</v>
-      </c>
       <c r="X8">
         <f t="shared" si="1"/>
-        <v>750</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
@@ -819,79 +797,79 @@
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
+        <v>450000</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>225000</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
         <v>112500</v>
       </c>
-      <c r="G9">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>64285.714285714283</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>56250</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>37500</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>28125</v>
-      </c>
-      <c r="J9">
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>45000</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="0"/>
         <v>22500</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>18750</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>16071.428571428571</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>14062.5</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>12500</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>11250</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>5625</v>
-      </c>
       <c r="Q9">
         <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
         <v>3750</v>
       </c>
-      <c r="R9">
-        <f t="shared" si="0"/>
+      <c r="V9">
+        <f t="shared" si="1"/>
         <v>2250</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
+      <c r="W9">
+        <f t="shared" si="1"/>
         <v>1875</v>
       </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
-        <v>1125</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="0"/>
-        <v>937.5</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="1"/>
-        <v>562.5</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="1"/>
-        <v>468.75</v>
-      </c>
       <c r="X9">
         <f t="shared" si="1"/>
-        <v>375</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
@@ -904,79 +882,79 @@
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
+        <v>225000</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>112500</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
         <v>56250</v>
       </c>
-      <c r="G10">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>45000</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>37500</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>32142.857142857141</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>28125</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>18750</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>14062.5</v>
-      </c>
-      <c r="J10">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>22500</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="0"/>
         <v>11250</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>9375</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>8035.7142857142853</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>7031.25</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="0"/>
-        <v>6250</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>5625</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>2812.5</v>
-      </c>
       <c r="Q10">
         <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>4500</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
         <v>1875</v>
       </c>
-      <c r="R10">
-        <f t="shared" si="0"/>
+      <c r="V10">
+        <f t="shared" si="1"/>
         <v>1125</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="0"/>
+      <c r="W10">
+        <f t="shared" si="1"/>
         <v>937.5</v>
       </c>
-      <c r="T10">
-        <f t="shared" si="0"/>
-        <v>562.5</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="0"/>
-        <v>468.75</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="1"/>
-        <v>281.25</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="1"/>
-        <v>234.375</v>
-      </c>
       <c r="X10">
         <f t="shared" si="1"/>
-        <v>187.5</v>
+        <v>750</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
@@ -989,79 +967,79 @@
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
+        <v>112500</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>56250</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>37500</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
         <v>28125</v>
       </c>
-      <c r="G11">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>22500</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>18750</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>16071.428571428571</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="0"/>
         <v>14062.5</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>9375</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>7031.25</v>
-      </c>
-      <c r="J11">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>12500</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>11250</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="0"/>
         <v>5625</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>4687.5</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>4017.8571428571427</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>3515.625</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="0"/>
-        <v>3125</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="0"/>
-        <v>2812.5</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>1406.25</v>
-      </c>
       <c r="Q11">
         <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>1875</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
         <v>937.5</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="0"/>
+      <c r="V11">
+        <f t="shared" si="1"/>
         <v>562.5</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
+      <c r="W11">
+        <f t="shared" si="1"/>
         <v>468.75</v>
       </c>
-      <c r="T11">
-        <f t="shared" si="0"/>
-        <v>281.25</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="0"/>
-        <v>234.375</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="1"/>
-        <v>140.625</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="1"/>
-        <v>117.1875</v>
-      </c>
       <c r="X11">
         <f t="shared" si="1"/>
-        <v>93.75</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="10:17" x14ac:dyDescent="0.25">

</xml_diff>